<commit_message>
Schematron updates for v3.5.1.250115: * Finalized version/build number * Updated all resources affected by element name changes
</commit_message>
<xml_diff>
--- a/Schematron/documentation/Schematron_3.5.0_3.5.1_Comparison.xlsx
+++ b/Schematron/documentation/Schematron_3.5.0_3.5.1_Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\NEMSIS TAC\Repository\nemsis_public\Schematron\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\NEMSIS TAC\Repository\nemsis\Schematron\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33509C44-6CB0-46A4-9F5D-510085B281D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E77CEE-22D0-4E94-BC90-07C5437E506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EFB0DDD4-CF85-4C10-9AFB-9B88D9ECAAEF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="406">
   <si>
     <t>…</t>
   </si>
@@ -1245,6 +1245,15 @@
   </si>
   <si>
     <t>3.5.1.240923 (candidate release)</t>
+  </si>
+  <si>
+    <t>3.5.1.250115</t>
+  </si>
+  <si>
+    <t>Date/Time Last Known Well should be recorded when Patient Evaluation/Care is "Patient Evaluated and Care Provided" and Stroke Scale Result is "Positive".</t>
+  </si>
+  <si>
+    <t>Hospital Capability should be recorded when Type of Destination is "Hospital..." or "Freestanding Emergency Department" and Stroke Scale Result is "Positive".</t>
   </si>
 </sst>
 </file>
@@ -1296,7 +1305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1311,6 +1320,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1526,8 +1538,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{556D836C-5BB8-4363-A43F-03102515214D}" name="EMSDataSet" displayName="EMSDataSet" ref="A3:G195" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
-  <autoFilter ref="A3:G195" xr:uid="{D5FB1F5A-F1E9-47F6-9AE4-2715FA1AD725}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{556D836C-5BB8-4363-A43F-03102515214D}" name="EMSDataSet" displayName="EMSDataSet" ref="A3:G200" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A3:G200" xr:uid="{D5FB1F5A-F1E9-47F6-9AE4-2715FA1AD725}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{32D489DB-6EFA-44A6-8581-B457388CB8F8}" name="3.5.0 ID" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{6C4001B3-37AD-4F9A-B826-F8D3DEB43335}" name="3.5.0 Level" dataDxfId="29"/>
@@ -1906,7 +1918,7 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -3744,7 +3756,7 @@
         <v>1</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>279</v>
+        <v>404</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -5444,7 +5456,7 @@
         <v>1</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>362</v>
+        <v>405</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -5748,6 +5760,7 @@
       </c>
     </row>
     <row r="196" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A196" s="6"/>
       <c r="E196" s="1" t="s">
         <v>392</v>
       </c>
@@ -5759,6 +5772,7 @@
       </c>
     </row>
     <row r="197" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A197" s="6"/>
       <c r="E197" s="1" t="s">
         <v>393</v>
       </c>
@@ -5770,6 +5784,7 @@
       </c>
     </row>
     <row r="198" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A198" s="6"/>
       <c r="E198" s="1" t="s">
         <v>394</v>
       </c>
@@ -5781,6 +5796,7 @@
       </c>
     </row>
     <row r="199" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A199" s="6"/>
       <c r="E199" s="1" t="s">
         <v>395</v>
       </c>
@@ -5792,6 +5808,7 @@
       </c>
     </row>
     <row r="200" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A200" s="6"/>
       <c r="E200" s="1" t="s">
         <v>396</v>
       </c>

</xml_diff>

<commit_message>
Updated National Schematron Rules Comparison (v3.5.0 to v3.5.1) for v3.5.0.250403CP5 and v3.5.1.250403CP1.
</commit_message>
<xml_diff>
--- a/Schematron/documentation/Schematron_3.5.0_3.5.1_Comparison.xlsx
+++ b/Schematron/documentation/Schematron_3.5.0_3.5.1_Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\NEMSIS TAC\Repository\nemsis\Schematron\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\NEMSIS TAC\Repository\nemsis_public\Schematron\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E77CEE-22D0-4E94-BC90-07C5437E506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D78278D-F68C-4D05-95B2-5988F0EDC97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EFB0DDD4-CF85-4C10-9AFB-9B88D9ECAAEF}"/>
   </bookViews>
@@ -233,9 +233,6 @@
     <t>nemSch_e060</t>
   </si>
   <si>
-    <t>nemSch_e061</t>
-  </si>
-  <si>
     <t>nemSch_e062</t>
   </si>
   <si>
@@ -800,9 +797,6 @@
     <t>Patient's Home ZIP Code should be recorded when Patient Evaluation/Care is "Patient Evaluated and Care Provided".</t>
   </si>
   <si>
-    <t>Gender should be recorded when Patient Evaluation/Care is "Patient Evaluated and Care Provided".</t>
-  </si>
-  <si>
     <t>Race should be recorded when Patient Evaluation/Care is "Patient Evaluated and Care Provided".</t>
   </si>
   <si>
@@ -1178,9 +1172,6 @@
     <t>Trauma Triage Criteria (Moderate Risk for Serious Injury) should only be recorded when Possible Injury is "Yes".</t>
   </si>
   <si>
-    <t>3.5.0.230317CP4</t>
-  </si>
-  <si>
     <t>3.5.0 ID</t>
   </si>
   <si>
@@ -1244,16 +1235,25 @@
     <t>When Date/Time of Cardiac Arrest has a Pertinent Negative of "Approximate", it should have a value and it should not have a Not Value (Not Applicable, Not Recorded, or Not Reporting).</t>
   </si>
   <si>
-    <t>3.5.1.240923 (candidate release)</t>
-  </si>
-  <si>
-    <t>3.5.1.250115</t>
-  </si>
-  <si>
     <t>Date/Time Last Known Well should be recorded when Patient Evaluation/Care is "Patient Evaluated and Care Provided" and Stroke Scale Result is "Positive".</t>
   </si>
   <si>
     <t>Hospital Capability should be recorded when Type of Destination is "Hospital..." or "Freestanding Emergency Department" and Stroke Scale Result is "Positive".</t>
+  </si>
+  <si>
+    <t>nemSch_e193</t>
+  </si>
+  <si>
+    <t>Sex should be recorded when Patient Evaluation/Care is "Patient Evaluated and Care Provided".</t>
+  </si>
+  <si>
+    <t>3.5.0.250403CP5</t>
+  </si>
+  <si>
+    <t>3.5.1.250403CP1</t>
+  </si>
+  <si>
+    <t>National Schematron Rules Comparison for EMSDataSet</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1320,9 +1320,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1882,7 +1879,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DB0597-B734-4DDE-A8D8-647079D1FCD6}">
-  <dimension ref="A1:G200"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -1902,7 +1899,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1913,37 +1910,37 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1954,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -1963,7 +1960,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1994,7 +1991,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
@@ -2003,7 +2000,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2014,7 +2011,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
@@ -2023,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2074,7 +2071,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -2083,7 +2080,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2094,7 +2091,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>6</v>
@@ -2103,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -2114,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
@@ -2123,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -2134,7 +2131,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>8</v>
@@ -2143,7 +2140,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2154,7 +2151,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>9</v>
@@ -2163,7 +2160,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2174,7 +2171,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>10</v>
@@ -2183,7 +2180,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2194,7 +2191,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
@@ -2203,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2214,7 +2211,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
@@ -2223,7 +2220,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2234,7 +2231,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
@@ -2243,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2254,7 +2251,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>14</v>
@@ -2263,7 +2260,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2274,7 +2271,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>15</v>
@@ -2283,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2294,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
@@ -2303,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2314,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -2323,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2334,7 +2331,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>18</v>
@@ -2343,7 +2340,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2354,7 +2351,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>19</v>
@@ -2363,7 +2360,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2374,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>20</v>
@@ -2383,7 +2380,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2394,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>21</v>
@@ -2403,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2414,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>22</v>
@@ -2423,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2434,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>23</v>
@@ -2443,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2454,7 +2451,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>24</v>
@@ -2463,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2474,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>25</v>
@@ -2483,7 +2480,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2494,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>26</v>
@@ -2503,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2514,7 +2511,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>27</v>
@@ -2523,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2534,7 +2531,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>28</v>
@@ -2543,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2554,7 +2551,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>29</v>
@@ -2563,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2574,7 +2571,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>30</v>
@@ -2583,7 +2580,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2594,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>31</v>
@@ -2603,7 +2600,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2614,7 +2611,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>32</v>
@@ -2623,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2634,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>33</v>
@@ -2643,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2654,7 +2651,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>34</v>
@@ -2663,7 +2660,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2674,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>35</v>
@@ -2683,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2694,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>36</v>
@@ -2703,7 +2700,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2714,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>37</v>
@@ -2723,7 +2720,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2734,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>38</v>
@@ -2743,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2754,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>39</v>
@@ -2763,7 +2760,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -2774,7 +2771,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>40</v>
@@ -2783,7 +2780,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2794,7 +2791,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>41</v>
@@ -2803,7 +2800,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2814,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>42</v>
@@ -2823,7 +2820,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2834,7 +2831,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>43</v>
@@ -2843,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2854,7 +2851,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>44</v>
@@ -2863,7 +2860,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2874,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>45</v>
@@ -2883,7 +2880,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2894,7 +2891,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>46</v>
@@ -2903,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2914,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>47</v>
@@ -2923,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2934,7 +2931,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>48</v>
@@ -2943,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2954,7 +2951,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>49</v>
@@ -2963,7 +2960,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2974,7 +2971,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>50</v>
@@ -2983,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2994,7 +2991,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>51</v>
@@ -3003,7 +3000,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3014,7 +3011,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>52</v>
@@ -3023,7 +3020,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3034,7 +3031,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>53</v>
@@ -3043,7 +3040,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3054,7 +3051,7 @@
         <v>1</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>54</v>
@@ -3063,7 +3060,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3074,7 +3071,7 @@
         <v>1</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>55</v>
@@ -3083,7 +3080,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3094,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>56</v>
@@ -3103,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3114,7 +3111,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>57</v>
@@ -3123,7 +3120,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3134,7 +3131,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>58</v>
@@ -3143,7 +3140,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3154,7 +3151,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>59</v>
@@ -3163,7 +3160,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -3174,7 +3171,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>60</v>
@@ -3183,7 +3180,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3194,7 +3191,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>61</v>
@@ -3203,7 +3200,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3214,7 +3211,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>62</v>
@@ -3223,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3234,7 +3231,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>63</v>
@@ -3243,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -3254,7 +3251,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>64</v>
@@ -3263,2560 +3260,2555 @@
         <v>1</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G126" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G139" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G140" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="182" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F192" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="194" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="195" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A196" s="6"/>
       <c r="E196" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="197" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A197" s="6"/>
       <c r="E197" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A198" s="6"/>
       <c r="E198" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="199" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A199" s="6"/>
       <c r="E199" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A200" s="6"/>
       <c r="E200" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G200" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
         <v>401</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -5825,12 +5817,12 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:G2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A4:C200">
+  <conditionalFormatting sqref="A4:C69 A71:C201">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="notEqual">
       <formula>E4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:G200">
+  <conditionalFormatting sqref="E4:G69 E71:G201">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="notEqual">
       <formula>A4</formula>
     </cfRule>
@@ -5865,7 +5857,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -5876,42 +5868,42 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3"/>
@@ -5968,7 +5960,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -5979,42 +5971,42 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3"/>

</xml_diff>